<commit_message>
Update tracking for inventory sheet
</commit_message>
<xml_diff>
--- a/input/Inventory sheet v2 - Grain.xlsx
+++ b/input/Inventory sheet v2 - Grain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\vinh\Git\File-Sharing\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73534CA1-9503-468C-B414-91B3F5159166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A42BD9B-BDB5-4E75-A9B7-98D64F82E8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="781" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="781" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General information" sheetId="6" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Chemical compounds" sheetId="3" r:id="rId12"/>
     <sheet name="Fuel Formula &amp; Constant" sheetId="15" r:id="rId13"/>
     <sheet name="Raw table (Hide)" sheetId="16" state="hidden" r:id="rId14"/>
-    <sheet name="Lookup Value (HIDE)" sheetId="13" r:id="rId15"/>
+    <sheet name="Lookup Value (HIDE)" sheetId="13" state="hidden" r:id="rId15"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Chemical compounds'!$A$1:$O$1</definedName>
@@ -543,7 +543,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1510" uniqueCount="911">
   <si>
     <t>Type</t>
   </si>
@@ -3273,9 +3273,6 @@
   </si>
   <si>
     <t>LPG Allocation (L)_GAFF</t>
-  </si>
-  <si>
-    <t>times</t>
   </si>
   <si>
     <t>Times</t>
@@ -6655,7 +6652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B3EC77-B402-48B7-8DD7-F4CAD2D0731E}">
   <dimension ref="A1:N319"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A97" workbookViewId="0">
+    <sheetView showZeros="0" workbookViewId="0">
       <selection activeCell="A201" sqref="A201:F201"/>
     </sheetView>
   </sheetViews>
@@ -17080,7 +17077,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17146,7 +17143,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I2" s="27">
-        <f>F2*G2</f>
+        <f>F2*G2*H2</f>
         <v>0</v>
       </c>
       <c r="J2" s="27">
@@ -17178,7 +17175,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I3" s="27">
-        <f t="shared" ref="I3:I54" si="0">F3*G3</f>
+        <f t="shared" ref="I3:I54" si="0">F3*G3*H3</f>
         <v>0</v>
       </c>
       <c r="J3" s="27">
@@ -18825,7 +18822,7 @@
           <x14:formula1>
             <xm:f>'Fert Comp'!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A54</xm:sqref>
+          <xm:sqref>A3:A54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -18838,7 +18835,7 @@
   <dimension ref="A1:V326"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18920,7 +18917,7 @@
         <v>257</v>
       </c>
       <c r="S1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="T1" t="s">
         <v>255</v>
@@ -18941,6 +18938,18 @@
         <f t="array" ref="D2">IFERROR(VLOOKUP(A2,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
       </c>
+      <c r="T2">
+        <f>$Q2*$R2*$S2*IF(F2=0,G2,F2)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <f>$Q2*$R2*$S2*IF(J2=0,K2,J2)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <f>$Q2*$R2*$S2*IF(N2=0,O2,N2)/1000</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C3" t="str">
@@ -18952,15 +18961,15 @@
         <v/>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T66" si="0">IF(G3=0,F3*Q3*R3,G3*Q3*R3)/1000</f>
+        <f t="shared" ref="T3:T66" si="0">$Q3*$R3*$S3*IF(F3=0,G3,F3)/1000</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U66" si="1">IF(K3=0,J3*Q3*R3,K3*Q3*R3)/1000</f>
+        <f t="shared" ref="U3:U66" si="1">$Q3*$R3*$S3*IF(J3=0,K3,J3)/1000</f>
         <v>0</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V52" si="2">IF(O3=0,N3*Q3*R3,O3*Q3*R3)/1000</f>
+        <f t="shared" ref="V3:V66" si="2">$Q3*$R3*$S3*IF(N3=0,O3,N3)/1000</f>
         <v>0</v>
       </c>
     </row>
@@ -20059,6 +20068,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V53">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C54" t="str">
@@ -20077,6 +20090,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D55" t="str" cm="1">
@@ -20091,6 +20108,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V55">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D56" t="str" cm="1">
@@ -20105,6 +20126,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V56">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D57" t="str" cm="1">
@@ -20119,6 +20144,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V57">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D58" t="str" cm="1">
@@ -20133,6 +20162,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V58">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D59" t="str" cm="1">
@@ -20147,6 +20180,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V59">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D60" t="str" cm="1">
@@ -20161,6 +20198,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V60">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D61" t="str" cm="1">
@@ -20175,6 +20216,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V61">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D62" t="str" cm="1">
@@ -20189,6 +20234,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D63" t="str" cm="1">
@@ -20203,6 +20252,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D64" t="str" cm="1">
@@ -20217,8 +20270,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V64">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D65" t="str" cm="1">
         <f t="array" ref="D65">IFERROR(VLOOKUP(A65,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20231,8 +20288,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V65">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D66" t="str" cm="1">
         <f t="array" ref="D66">IFERROR(VLOOKUP(A66,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20245,22 +20306,30 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V66">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D67" t="str" cm="1">
         <f t="array" ref="D67">IFERROR(VLOOKUP(A67,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
       </c>
       <c r="T67">
-        <f t="shared" ref="T67:T130" si="3">IF(G67=0,F67*Q67*R67,G67*Q67*R67)/1000</f>
+        <f t="shared" ref="T67:T130" si="3">$Q67*$R67*$S67*IF(F67=0,G67,F67)/1000</f>
         <v>0</v>
       </c>
       <c r="U67">
-        <f t="shared" ref="U67:U130" si="4">IF(K67=0,J67*Q67*R67,K67*Q67*R67)/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U67:U130" si="4">$Q67*$R67*$S67*IF(J67=0,K67,J67)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="V67">
+        <f t="shared" ref="V67:V130" si="5">$Q67*$R67*$S67*IF(N67=0,O67,N67)/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D68" t="str" cm="1">
         <f t="array" ref="D68">IFERROR(VLOOKUP(A68,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20273,8 +20342,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V68">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D69" t="str" cm="1">
         <f t="array" ref="D69">IFERROR(VLOOKUP(A69,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20287,8 +20360,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V69">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D70" t="str" cm="1">
         <f t="array" ref="D70">IFERROR(VLOOKUP(A70,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20301,8 +20378,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V70">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D71" t="str" cm="1">
         <f t="array" ref="D71">IFERROR(VLOOKUP(A71,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20315,8 +20396,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V71">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D72" t="str" cm="1">
         <f t="array" ref="D72">IFERROR(VLOOKUP(A72,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20329,8 +20414,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V72">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D73" t="str" cm="1">
         <f t="array" ref="D73">IFERROR(VLOOKUP(A73,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20343,8 +20432,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V73">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D74" t="str" cm="1">
         <f t="array" ref="D74">IFERROR(VLOOKUP(A74,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20357,8 +20450,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V74">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D75" t="str" cm="1">
         <f t="array" ref="D75">IFERROR(VLOOKUP(A75,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20371,8 +20468,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V75">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D76" t="str" cm="1">
         <f t="array" ref="D76">IFERROR(VLOOKUP(A76,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20385,8 +20486,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V76">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D77" t="str" cm="1">
         <f t="array" ref="D77">IFERROR(VLOOKUP(A77,'Chemical compounds'!$A$1:$O$294,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20399,8 +20504,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V77">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D78" t="str" cm="1">
         <f t="array" ref="D78">IFERROR(VLOOKUP(A78,'Chemical compounds'!A76:O370,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20413,8 +20522,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V78">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D79" t="str" cm="1">
         <f t="array" ref="D79">IFERROR(VLOOKUP(A79,'Chemical compounds'!A77:O371,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20427,8 +20540,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V79">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D80" t="str" cm="1">
         <f t="array" ref="D80">IFERROR(VLOOKUP(A80,'Chemical compounds'!A78:O372,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20441,8 +20558,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V80">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D81" t="str" cm="1">
         <f t="array" ref="D81">IFERROR(VLOOKUP(A81,'Chemical compounds'!A79:O373,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20455,8 +20576,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V81">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D82" t="str" cm="1">
         <f t="array" ref="D82">IFERROR(VLOOKUP(A82,'Chemical compounds'!A80:O374,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20469,8 +20594,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V82">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D83" t="str" cm="1">
         <f t="array" ref="D83">IFERROR(VLOOKUP(A83,'Chemical compounds'!A81:O375,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20483,8 +20612,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V83">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D84" t="str" cm="1">
         <f t="array" ref="D84">IFERROR(VLOOKUP(A84,'Chemical compounds'!A82:O376,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20497,8 +20630,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V84">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D85" t="str" cm="1">
         <f t="array" ref="D85">IFERROR(VLOOKUP(A85,'Chemical compounds'!A83:O377,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20511,8 +20648,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V85">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D86" t="str" cm="1">
         <f t="array" ref="D86">IFERROR(VLOOKUP(A86,'Chemical compounds'!A84:O378,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20525,8 +20666,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V86">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D87" t="str" cm="1">
         <f t="array" ref="D87">IFERROR(VLOOKUP(A87,'Chemical compounds'!A85:O379,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20539,8 +20684,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V87">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D88" t="str" cm="1">
         <f t="array" ref="D88">IFERROR(VLOOKUP(A88,'Chemical compounds'!A86:O380,{2,3,4,5,6,7,8,9,10,11,12,13},0),"")</f>
         <v/>
@@ -20553,8 +20702,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V88">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D89" t="str" cm="1">
         <f t="array" ref="D89">IFERROR(VLOOKUP(A89,'Chemical compounds'!A87:O381,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20567,8 +20720,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V89">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D90" t="str" cm="1">
         <f t="array" ref="D90">IFERROR(VLOOKUP(A90,'Chemical compounds'!A88:O382,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20581,8 +20738,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V90">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D91" t="str" cm="1">
         <f t="array" ref="D91">IFERROR(VLOOKUP(A91,'Chemical compounds'!A89:O383,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20595,8 +20756,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V91">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D92" t="str" cm="1">
         <f t="array" ref="D92">IFERROR(VLOOKUP(A92,'Chemical compounds'!A90:O384,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20609,8 +20774,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V92">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D93" t="str" cm="1">
         <f t="array" ref="D93">IFERROR(VLOOKUP(A93,'Chemical compounds'!A91:O385,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20623,8 +20792,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V93">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D94" t="str" cm="1">
         <f t="array" ref="D94">IFERROR(VLOOKUP(A94,'Chemical compounds'!A92:O386,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20637,8 +20810,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V94">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D95" t="str" cm="1">
         <f t="array" ref="D95">IFERROR(VLOOKUP(A95,'Chemical compounds'!A93:O387,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20651,8 +20828,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V95">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D96" t="str" cm="1">
         <f t="array" ref="D96">IFERROR(VLOOKUP(A96,'Chemical compounds'!A94:O388,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20665,8 +20846,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V96">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D97" t="str" cm="1">
         <f t="array" ref="D97">IFERROR(VLOOKUP(A97,'Chemical compounds'!A95:O389,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20679,8 +20864,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V97">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D98" t="str" cm="1">
         <f t="array" ref="D98">IFERROR(VLOOKUP(A98,'Chemical compounds'!A96:O390,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20693,8 +20882,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V98">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D99" t="str" cm="1">
         <f t="array" ref="D99">IFERROR(VLOOKUP(A99,'Chemical compounds'!A97:O391,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20707,8 +20900,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V99">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D100" t="str" cm="1">
         <f t="array" ref="D100">IFERROR(VLOOKUP(A100,'Chemical compounds'!A98:O392,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20721,8 +20918,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V100">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D101" t="str" cm="1">
         <f t="array" ref="D101">IFERROR(VLOOKUP(A101,'Chemical compounds'!A99:O393,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20735,8 +20936,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V101">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D102" t="str" cm="1">
         <f t="array" ref="D102">IFERROR(VLOOKUP(A102,'Chemical compounds'!A100:O394,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20749,8 +20954,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V102">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D103" t="str" cm="1">
         <f t="array" ref="D103">IFERROR(VLOOKUP(A103,'Chemical compounds'!A101:O395,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20763,8 +20972,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V103">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D104" t="str" cm="1">
         <f t="array" ref="D104">IFERROR(VLOOKUP(A104,'Chemical compounds'!A102:O396,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20777,8 +20990,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V104">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D105" t="str" cm="1">
         <f t="array" ref="D105">IFERROR(VLOOKUP(A105,'Chemical compounds'!A103:O397,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20791,8 +21008,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V105">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D106" t="str" cm="1">
         <f t="array" ref="D106">IFERROR(VLOOKUP(A106,'Chemical compounds'!A104:O398,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20805,8 +21026,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V106">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D107" t="str" cm="1">
         <f t="array" ref="D107">IFERROR(VLOOKUP(A107,'Chemical compounds'!A105:O399,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20819,8 +21044,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V107">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D108" t="str" cm="1">
         <f t="array" ref="D108">IFERROR(VLOOKUP(A108,'Chemical compounds'!A106:O400,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20833,8 +21062,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V108">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D109" t="str" cm="1">
         <f t="array" ref="D109">IFERROR(VLOOKUP(A109,'Chemical compounds'!A107:O401,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20847,8 +21080,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V109">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D110" t="str" cm="1">
         <f t="array" ref="D110">IFERROR(VLOOKUP(A110,'Chemical compounds'!A108:O402,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20861,8 +21098,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="111" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V110">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D111" t="str" cm="1">
         <f t="array" ref="D111">IFERROR(VLOOKUP(A111,'Chemical compounds'!A109:O403,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20875,8 +21116,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="112" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V111">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D112" t="str" cm="1">
         <f t="array" ref="D112">IFERROR(VLOOKUP(A112,'Chemical compounds'!A110:O404,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20889,8 +21134,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="113" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V112">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D113" t="str" cm="1">
         <f t="array" ref="D113">IFERROR(VLOOKUP(A113,'Chemical compounds'!A111:O405,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20903,8 +21152,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="114" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V113">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D114" t="str" cm="1">
         <f t="array" ref="D114">IFERROR(VLOOKUP(A114,'Chemical compounds'!A112:O406,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20917,8 +21170,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="115" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V114">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D115" t="str" cm="1">
         <f t="array" ref="D115">IFERROR(VLOOKUP(A115,'Chemical compounds'!A113:O407,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20931,8 +21188,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="116" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V115">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D116" t="str" cm="1">
         <f t="array" ref="D116">IFERROR(VLOOKUP(A116,'Chemical compounds'!A114:O408,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20945,8 +21206,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="117" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V116">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D117" t="str" cm="1">
         <f t="array" ref="D117">IFERROR(VLOOKUP(A117,'Chemical compounds'!A115:O409,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20959,8 +21224,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V117">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D118" t="str" cm="1">
         <f t="array" ref="D118">IFERROR(VLOOKUP(A118,'Chemical compounds'!A116:O410,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20973,8 +21242,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V118">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D119" t="str" cm="1">
         <f t="array" ref="D119">IFERROR(VLOOKUP(A119,'Chemical compounds'!A117:O411,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -20987,8 +21260,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V119">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D120" t="str" cm="1">
         <f t="array" ref="D120">IFERROR(VLOOKUP(A120,'Chemical compounds'!A118:O412,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21001,8 +21278,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V120">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D121" t="str" cm="1">
         <f t="array" ref="D121">IFERROR(VLOOKUP(A121,'Chemical compounds'!A119:O413,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21015,8 +21296,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="122" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V121">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D122" t="str" cm="1">
         <f t="array" ref="D122">IFERROR(VLOOKUP(A122,'Chemical compounds'!A120:O414,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21029,8 +21314,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="123" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V122">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D123" t="str" cm="1">
         <f t="array" ref="D123">IFERROR(VLOOKUP(A123,'Chemical compounds'!A121:O415,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21043,8 +21332,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="124" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V123">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D124" t="str" cm="1">
         <f t="array" ref="D124">IFERROR(VLOOKUP(A124,'Chemical compounds'!A122:O416,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21057,8 +21350,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="125" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V124">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D125" t="str" cm="1">
         <f t="array" ref="D125">IFERROR(VLOOKUP(A125,'Chemical compounds'!A123:O417,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21071,8 +21368,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="126" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V125">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D126" t="str" cm="1">
         <f t="array" ref="D126">IFERROR(VLOOKUP(A126,'Chemical compounds'!A124:O418,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21085,8 +21386,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V126">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D127" t="str" cm="1">
         <f t="array" ref="D127">IFERROR(VLOOKUP(A127,'Chemical compounds'!A125:O419,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21099,8 +21404,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="128" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V127">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D128" t="str" cm="1">
         <f t="array" ref="D128">IFERROR(VLOOKUP(A128,'Chemical compounds'!A126:O420,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21113,8 +21422,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="129" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V128">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D129" t="str" cm="1">
         <f t="array" ref="D129">IFERROR(VLOOKUP(A129,'Chemical compounds'!A127:O421,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21127,8 +21440,12 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="130" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V129">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D130" t="str" cm="1">
         <f t="array" ref="D130">IFERROR(VLOOKUP(A130,'Chemical compounds'!A128:O422,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
@@ -21141,648 +21458,800 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="131" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="V130">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D131" t="str" cm="1">
         <f t="array" ref="D131">IFERROR(VLOOKUP(A131,'Chemical compounds'!A129:O423,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T131">
-        <f t="shared" ref="T131:T194" si="5">IF(G131=0,F131*Q131*R131,G131*Q131*R131)/1000</f>
+        <f t="shared" ref="T131:T167" si="6">$Q131*$R131*$S131*IF(F131=0,G131,F131)/1000</f>
         <v>0</v>
       </c>
       <c r="U131">
-        <f t="shared" ref="U131:U194" si="6">IF(K131=0,J131*Q131*R131,K131*Q131*R131)/1000</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U131:U167" si="7">$Q131*$R131*$S131*IF(J131=0,K131,J131)/1000</f>
+        <v>0</v>
+      </c>
+      <c r="V131">
+        <f t="shared" ref="V131:V167" si="8">$Q131*$R131*$S131*IF(N131=0,O131,N131)/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D132" t="str" cm="1">
         <f t="array" ref="D132">IFERROR(VLOOKUP(A132,'Chemical compounds'!A130:O424,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T132">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U132">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V132">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D133" t="str" cm="1">
         <f t="array" ref="D133">IFERROR(VLOOKUP(A133,'Chemical compounds'!A131:O425,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T133">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U133">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V133">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D134" t="str" cm="1">
         <f t="array" ref="D134">IFERROR(VLOOKUP(A134,'Chemical compounds'!A132:O426,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T134">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U134">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V134">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D135" t="str" cm="1">
         <f t="array" ref="D135">IFERROR(VLOOKUP(A135,'Chemical compounds'!A133:O427,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T135">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U135">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V135">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D136" t="str" cm="1">
         <f t="array" ref="D136">IFERROR(VLOOKUP(A136,'Chemical compounds'!A134:O428,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T136">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U136">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V136">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D137" t="str" cm="1">
         <f t="array" ref="D137">IFERROR(VLOOKUP(A137,'Chemical compounds'!A135:O429,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T137">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U137">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="138" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V137">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D138" t="str" cm="1">
         <f t="array" ref="D138">IFERROR(VLOOKUP(A138,'Chemical compounds'!A136:O430,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T138">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U138">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V138">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D139" t="str" cm="1">
         <f t="array" ref="D139">IFERROR(VLOOKUP(A139,'Chemical compounds'!A137:O431,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T139">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U139">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V139">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D140" t="str" cm="1">
         <f t="array" ref="D140">IFERROR(VLOOKUP(A140,'Chemical compounds'!A138:O432,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T140">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U140">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V140">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D141" t="str" cm="1">
         <f t="array" ref="D141">IFERROR(VLOOKUP(A141,'Chemical compounds'!A139:O433,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T141">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U141">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="142" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V141">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D142" t="str" cm="1">
         <f t="array" ref="D142">IFERROR(VLOOKUP(A142,'Chemical compounds'!A140:O434,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T142">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U142">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V142">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D143" t="str" cm="1">
         <f t="array" ref="D143">IFERROR(VLOOKUP(A143,'Chemical compounds'!A141:O435,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T143">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U143">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V143">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D144" t="str" cm="1">
         <f t="array" ref="D144">IFERROR(VLOOKUP(A144,'Chemical compounds'!A142:O436,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T144">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U144">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V144">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D145" t="str" cm="1">
         <f t="array" ref="D145">IFERROR(VLOOKUP(A145,'Chemical compounds'!A143:O437,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T145">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U145">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V145">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D146" t="str" cm="1">
         <f t="array" ref="D146">IFERROR(VLOOKUP(A146,'Chemical compounds'!A144:O438,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T146">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U146">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="147" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V146">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D147" t="str" cm="1">
         <f t="array" ref="D147">IFERROR(VLOOKUP(A147,'Chemical compounds'!A145:O439,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T147">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U147">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="148" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V147">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D148" t="str" cm="1">
         <f t="array" ref="D148">IFERROR(VLOOKUP(A148,'Chemical compounds'!A146:O440,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T148">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U148">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V148">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D149" t="str" cm="1">
         <f t="array" ref="D149">IFERROR(VLOOKUP(A149,'Chemical compounds'!A147:O441,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T149">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U149">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V149">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D150" t="str" cm="1">
         <f t="array" ref="D150">IFERROR(VLOOKUP(A150,'Chemical compounds'!A148:O442,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T150">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U150">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V150">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D151" t="str" cm="1">
         <f t="array" ref="D151">IFERROR(VLOOKUP(A151,'Chemical compounds'!A149:O443,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T151">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U151">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="152" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V151">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D152" t="str" cm="1">
         <f t="array" ref="D152">IFERROR(VLOOKUP(A152,'Chemical compounds'!A150:O444,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T152">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U152">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V152">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D153" t="str" cm="1">
         <f t="array" ref="D153">IFERROR(VLOOKUP(A153,'Chemical compounds'!A151:O445,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T153">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U153">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V153">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D154" t="str" cm="1">
         <f t="array" ref="D154">IFERROR(VLOOKUP(A154,'Chemical compounds'!A152:O446,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T154">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U154">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="155" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V154">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D155" t="str" cm="1">
         <f t="array" ref="D155">IFERROR(VLOOKUP(A155,'Chemical compounds'!A153:O447,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T155">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U155">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="156" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V155">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D156" t="str" cm="1">
         <f t="array" ref="D156">IFERROR(VLOOKUP(A156,'Chemical compounds'!A154:O448,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T156">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U156">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V156">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D157" t="str" cm="1">
         <f t="array" ref="D157">IFERROR(VLOOKUP(A157,'Chemical compounds'!A155:O449,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T157">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U157">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V157">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D158" t="str" cm="1">
         <f t="array" ref="D158">IFERROR(VLOOKUP(A158,'Chemical compounds'!A156:O450,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T158">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U158">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V158">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D159" t="str" cm="1">
         <f t="array" ref="D159">IFERROR(VLOOKUP(A159,'Chemical compounds'!A157:O451,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T159">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U159">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V159">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D160" t="str" cm="1">
         <f t="array" ref="D160">IFERROR(VLOOKUP(A160,'Chemical compounds'!A158:O452,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T160">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U160">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V160">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D161" t="str" cm="1">
         <f t="array" ref="D161">IFERROR(VLOOKUP(A161,'Chemical compounds'!A159:O453,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T161">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U161">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V161">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D162" t="str" cm="1">
         <f t="array" ref="D162">IFERROR(VLOOKUP(A162,'Chemical compounds'!A160:O454,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T162">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U162">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V162">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D163" t="str" cm="1">
         <f t="array" ref="D163">IFERROR(VLOOKUP(A163,'Chemical compounds'!A161:O455,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T163">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U163">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V163">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D164" t="str" cm="1">
         <f t="array" ref="D164">IFERROR(VLOOKUP(A164,'Chemical compounds'!A162:O456,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T164">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U164">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V164">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D165" t="str" cm="1">
         <f t="array" ref="D165">IFERROR(VLOOKUP(A165,'Chemical compounds'!A163:O457,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T165">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U165">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V165">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D166" t="str" cm="1">
         <f t="array" ref="D166">IFERROR(VLOOKUP(A166,'Chemical compounds'!A164:O458,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T166">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U166">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V166">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D167" t="str" cm="1">
         <f t="array" ref="D167">IFERROR(VLOOKUP(A167,'Chemical compounds'!A165:O459,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T167">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="U167">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="V167">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D168" t="str" cm="1">
         <f t="array" ref="D168">IFERROR(VLOOKUP(A168,'Chemical compounds'!A166:O460,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T168">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="T131:T194" si="9">IF(G168=0,F168*Q168*R168,G168*Q168*R168)/1000</f>
         <v>0</v>
       </c>
       <c r="U168">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" ref="U131:U194" si="10">IF(K168=0,J168*Q168*R168,K168*Q168*R168)/1000</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D169" t="str" cm="1">
         <f t="array" ref="D169">IFERROR(VLOOKUP(A169,'Chemical compounds'!A167:O461,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T169">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U169">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D170" t="str" cm="1">
         <f t="array" ref="D170">IFERROR(VLOOKUP(A170,'Chemical compounds'!A168:O462,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T170">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U170">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D171" t="str" cm="1">
         <f t="array" ref="D171">IFERROR(VLOOKUP(A171,'Chemical compounds'!A169:O463,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T171">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U171">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="172" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D172" t="str" cm="1">
         <f t="array" ref="D172">IFERROR(VLOOKUP(A172,'Chemical compounds'!A170:O464,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T172">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U172">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D173" t="str" cm="1">
         <f t="array" ref="D173">IFERROR(VLOOKUP(A173,'Chemical compounds'!A171:O465,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T173">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U173">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D174" t="str" cm="1">
         <f t="array" ref="D174">IFERROR(VLOOKUP(A174,'Chemical compounds'!A172:O466,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T174">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U174">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D175" t="str" cm="1">
         <f t="array" ref="D175">IFERROR(VLOOKUP(A175,'Chemical compounds'!A173:O467,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T175">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U175">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="4:21" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D176" t="str" cm="1">
         <f t="array" ref="D176">IFERROR(VLOOKUP(A176,'Chemical compounds'!A174:O468,{2,3,4,5,6,7,8,9},0),"")</f>
         <v/>
       </c>
       <c r="T176">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U176">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21792,11 +22261,11 @@
         <v/>
       </c>
       <c r="T177">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U177">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21806,11 +22275,11 @@
         <v/>
       </c>
       <c r="T178">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U178">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21820,11 +22289,11 @@
         <v/>
       </c>
       <c r="T179">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U179">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21834,11 +22303,11 @@
         <v/>
       </c>
       <c r="T180">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U180">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21848,11 +22317,11 @@
         <v/>
       </c>
       <c r="T181">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U181">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21862,11 +22331,11 @@
         <v/>
       </c>
       <c r="T182">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U182">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21876,11 +22345,11 @@
         <v/>
       </c>
       <c r="T183">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U183">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21890,11 +22359,11 @@
         <v/>
       </c>
       <c r="T184">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U184">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21904,11 +22373,11 @@
         <v/>
       </c>
       <c r="T185">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U185">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21918,11 +22387,11 @@
         <v/>
       </c>
       <c r="T186">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U186">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21932,11 +22401,11 @@
         <v/>
       </c>
       <c r="T187">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U187">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21946,11 +22415,11 @@
         <v/>
       </c>
       <c r="T188">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U188">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21960,11 +22429,11 @@
         <v/>
       </c>
       <c r="T189">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U189">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21974,11 +22443,11 @@
         <v/>
       </c>
       <c r="T190">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U190">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -21988,11 +22457,11 @@
         <v/>
       </c>
       <c r="T191">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U191">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -22002,11 +22471,11 @@
         <v/>
       </c>
       <c r="T192">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U192">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -22016,11 +22485,11 @@
         <v/>
       </c>
       <c r="T193">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U193">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -22030,11 +22499,11 @@
         <v/>
       </c>
       <c r="T194">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="U194">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -22044,11 +22513,11 @@
         <v/>
       </c>
       <c r="T195">
-        <f t="shared" ref="T195:T258" si="7">IF(G195=0,F195*Q195*R195,G195*Q195*R195)/1000</f>
+        <f t="shared" ref="T195:T258" si="11">IF(G195=0,F195*Q195*R195,G195*Q195*R195)/1000</f>
         <v>0</v>
       </c>
       <c r="U195">
-        <f t="shared" ref="U195:U258" si="8">IF(K195=0,J195*Q195*R195,K195*Q195*R195)/1000</f>
+        <f t="shared" ref="U195:U258" si="12">IF(K195=0,J195*Q195*R195,K195*Q195*R195)/1000</f>
         <v>0</v>
       </c>
     </row>
@@ -22058,11 +22527,11 @@
         <v/>
       </c>
       <c r="T196">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U196">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22072,11 +22541,11 @@
         <v/>
       </c>
       <c r="T197">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U197">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22086,11 +22555,11 @@
         <v/>
       </c>
       <c r="T198">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U198">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22100,11 +22569,11 @@
         <v/>
       </c>
       <c r="T199">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U199">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22114,11 +22583,11 @@
         <v/>
       </c>
       <c r="T200">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U200">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22128,11 +22597,11 @@
         <v/>
       </c>
       <c r="T201">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U201">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22142,11 +22611,11 @@
         <v/>
       </c>
       <c r="T202">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U202">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22156,11 +22625,11 @@
         <v/>
       </c>
       <c r="T203">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U203">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22170,11 +22639,11 @@
         <v/>
       </c>
       <c r="T204">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U204">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22184,11 +22653,11 @@
         <v/>
       </c>
       <c r="T205">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U205">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22198,11 +22667,11 @@
         <v/>
       </c>
       <c r="T206">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U206">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22212,11 +22681,11 @@
         <v/>
       </c>
       <c r="T207">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U207">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22226,11 +22695,11 @@
         <v/>
       </c>
       <c r="T208">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U208">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22240,11 +22709,11 @@
         <v/>
       </c>
       <c r="T209">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U209">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22254,11 +22723,11 @@
         <v/>
       </c>
       <c r="T210">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U210">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22268,11 +22737,11 @@
         <v/>
       </c>
       <c r="T211">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U211">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22282,11 +22751,11 @@
         <v/>
       </c>
       <c r="T212">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U212">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22296,11 +22765,11 @@
         <v/>
       </c>
       <c r="T213">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U213">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22310,11 +22779,11 @@
         <v/>
       </c>
       <c r="T214">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U214">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22324,11 +22793,11 @@
         <v/>
       </c>
       <c r="T215">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U215">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22338,11 +22807,11 @@
         <v/>
       </c>
       <c r="T216">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U216">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22352,11 +22821,11 @@
         <v/>
       </c>
       <c r="T217">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U217">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22366,11 +22835,11 @@
         <v/>
       </c>
       <c r="T218">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U218">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22380,11 +22849,11 @@
         <v/>
       </c>
       <c r="T219">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U219">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22394,11 +22863,11 @@
         <v/>
       </c>
       <c r="T220">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U220">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22408,11 +22877,11 @@
         <v/>
       </c>
       <c r="T221">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U221">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22422,11 +22891,11 @@
         <v/>
       </c>
       <c r="T222">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U222">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22436,11 +22905,11 @@
         <v/>
       </c>
       <c r="T223">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U223">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22450,11 +22919,11 @@
         <v/>
       </c>
       <c r="T224">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U224">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22464,11 +22933,11 @@
         <v/>
       </c>
       <c r="T225">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U225">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22478,11 +22947,11 @@
         <v/>
       </c>
       <c r="T226">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U226">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22492,11 +22961,11 @@
         <v/>
       </c>
       <c r="T227">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U227">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22506,11 +22975,11 @@
         <v/>
       </c>
       <c r="T228">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U228">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22520,11 +22989,11 @@
         <v/>
       </c>
       <c r="T229">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U229">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22534,11 +23003,11 @@
         <v/>
       </c>
       <c r="T230">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U230">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22548,11 +23017,11 @@
         <v/>
       </c>
       <c r="T231">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U231">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22562,11 +23031,11 @@
         <v/>
       </c>
       <c r="T232">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U232">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22576,11 +23045,11 @@
         <v/>
       </c>
       <c r="T233">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U233">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22590,11 +23059,11 @@
         <v/>
       </c>
       <c r="T234">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U234">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22604,11 +23073,11 @@
         <v/>
       </c>
       <c r="T235">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U235">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22618,11 +23087,11 @@
         <v/>
       </c>
       <c r="T236">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U236">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22632,11 +23101,11 @@
         <v/>
       </c>
       <c r="T237">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U237">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22646,11 +23115,11 @@
         <v/>
       </c>
       <c r="T238">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U238">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22660,11 +23129,11 @@
         <v/>
       </c>
       <c r="T239">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U239">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22674,11 +23143,11 @@
         <v/>
       </c>
       <c r="T240">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U240">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22688,11 +23157,11 @@
         <v/>
       </c>
       <c r="T241">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U241">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22702,11 +23171,11 @@
         <v/>
       </c>
       <c r="T242">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U242">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22716,11 +23185,11 @@
         <v/>
       </c>
       <c r="T243">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U243">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22730,11 +23199,11 @@
         <v/>
       </c>
       <c r="T244">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U244">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22744,11 +23213,11 @@
         <v/>
       </c>
       <c r="T245">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U245">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22758,11 +23227,11 @@
         <v/>
       </c>
       <c r="T246">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U246">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22772,11 +23241,11 @@
         <v/>
       </c>
       <c r="T247">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U247">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22786,11 +23255,11 @@
         <v/>
       </c>
       <c r="T248">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U248">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22800,11 +23269,11 @@
         <v/>
       </c>
       <c r="T249">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U249">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22814,11 +23283,11 @@
         <v/>
       </c>
       <c r="T250">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U250">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22828,11 +23297,11 @@
         <v/>
       </c>
       <c r="T251">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U251">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22842,11 +23311,11 @@
         <v/>
       </c>
       <c r="T252">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U252">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22856,11 +23325,11 @@
         <v/>
       </c>
       <c r="T253">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U253">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22870,11 +23339,11 @@
         <v/>
       </c>
       <c r="T254">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U254">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22884,11 +23353,11 @@
         <v/>
       </c>
       <c r="T255">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U255">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22898,11 +23367,11 @@
         <v/>
       </c>
       <c r="T256">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U256">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22912,11 +23381,11 @@
         <v/>
       </c>
       <c r="T257">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U257">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22926,11 +23395,11 @@
         <v/>
       </c>
       <c r="T258">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="U258">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
     </row>
@@ -22940,11 +23409,11 @@
         <v/>
       </c>
       <c r="T259">
-        <f t="shared" ref="T259:T320" si="9">IF(G259=0,F259*Q259*R259,G259*Q259*R259)/1000</f>
+        <f t="shared" ref="T259:T320" si="13">IF(G259=0,F259*Q259*R259,G259*Q259*R259)/1000</f>
         <v>0</v>
       </c>
       <c r="U259">
-        <f t="shared" ref="U259:U320" si="10">IF(K259=0,J259*Q259*R259,K259*Q259*R259)/1000</f>
+        <f t="shared" ref="U259:U320" si="14">IF(K259=0,J259*Q259*R259,K259*Q259*R259)/1000</f>
         <v>0</v>
       </c>
     </row>
@@ -22954,11 +23423,11 @@
         <v/>
       </c>
       <c r="T260">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U260">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -22968,11 +23437,11 @@
         <v/>
       </c>
       <c r="T261">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U261">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -22982,11 +23451,11 @@
         <v/>
       </c>
       <c r="T262">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U262">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -22996,11 +23465,11 @@
         <v/>
       </c>
       <c r="T263">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U263">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23010,11 +23479,11 @@
         <v/>
       </c>
       <c r="T264">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U264">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23024,11 +23493,11 @@
         <v/>
       </c>
       <c r="T265">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U265">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23038,11 +23507,11 @@
         <v/>
       </c>
       <c r="T266">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U266">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23052,11 +23521,11 @@
         <v/>
       </c>
       <c r="T267">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U267">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23066,11 +23535,11 @@
         <v/>
       </c>
       <c r="T268">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U268">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23080,11 +23549,11 @@
         <v/>
       </c>
       <c r="T269">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U269">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23094,11 +23563,11 @@
         <v/>
       </c>
       <c r="T270">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U270">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23108,11 +23577,11 @@
         <v/>
       </c>
       <c r="T271">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U271">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23122,11 +23591,11 @@
         <v/>
       </c>
       <c r="T272">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U272">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23136,11 +23605,11 @@
         <v/>
       </c>
       <c r="T273">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U273">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23150,11 +23619,11 @@
         <v/>
       </c>
       <c r="T274">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U274">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23164,11 +23633,11 @@
         <v/>
       </c>
       <c r="T275">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U275">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23178,11 +23647,11 @@
         <v/>
       </c>
       <c r="T276">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U276">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23192,11 +23661,11 @@
         <v/>
       </c>
       <c r="T277">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U277">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23206,11 +23675,11 @@
         <v/>
       </c>
       <c r="T278">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U278">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23220,11 +23689,11 @@
         <v/>
       </c>
       <c r="T279">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U279">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23234,11 +23703,11 @@
         <v/>
       </c>
       <c r="T280">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U280">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23248,11 +23717,11 @@
         <v/>
       </c>
       <c r="T281">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U281">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23262,11 +23731,11 @@
         <v/>
       </c>
       <c r="T282">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U282">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23276,11 +23745,11 @@
         <v/>
       </c>
       <c r="T283">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U283">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23290,11 +23759,11 @@
         <v/>
       </c>
       <c r="T284">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U284">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23304,11 +23773,11 @@
         <v/>
       </c>
       <c r="T285">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U285">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23318,11 +23787,11 @@
         <v/>
       </c>
       <c r="T286">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U286">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23332,11 +23801,11 @@
         <v/>
       </c>
       <c r="T287">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U287">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23346,11 +23815,11 @@
         <v/>
       </c>
       <c r="T288">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U288">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23360,11 +23829,11 @@
         <v/>
       </c>
       <c r="T289">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U289">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23374,11 +23843,11 @@
         <v/>
       </c>
       <c r="T290">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U290">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23388,11 +23857,11 @@
         <v/>
       </c>
       <c r="T291">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U291">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23402,11 +23871,11 @@
         <v/>
       </c>
       <c r="T292">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U292">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23416,11 +23885,11 @@
         <v/>
       </c>
       <c r="T293">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U293">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23430,11 +23899,11 @@
         <v/>
       </c>
       <c r="T294">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U294">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23444,11 +23913,11 @@
         <v/>
       </c>
       <c r="T295">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U295">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23458,11 +23927,11 @@
         <v/>
       </c>
       <c r="T296">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U296">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23472,11 +23941,11 @@
         <v/>
       </c>
       <c r="T297">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U297">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23486,11 +23955,11 @@
         <v/>
       </c>
       <c r="T298">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U298">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23500,11 +23969,11 @@
         <v/>
       </c>
       <c r="T299">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U299">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23514,11 +23983,11 @@
         <v/>
       </c>
       <c r="T300">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U300">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23528,11 +23997,11 @@
         <v/>
       </c>
       <c r="T301">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U301">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23542,11 +24011,11 @@
         <v/>
       </c>
       <c r="T302">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U302">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23556,11 +24025,11 @@
         <v/>
       </c>
       <c r="T303">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U303">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23570,11 +24039,11 @@
         <v/>
       </c>
       <c r="T304">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U304">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23584,11 +24053,11 @@
         <v/>
       </c>
       <c r="T305">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U305">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23598,11 +24067,11 @@
         <v/>
       </c>
       <c r="T306">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U306">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23612,11 +24081,11 @@
         <v/>
       </c>
       <c r="T307">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U307">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23626,11 +24095,11 @@
         <v/>
       </c>
       <c r="T308">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U308">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23640,11 +24109,11 @@
         <v/>
       </c>
       <c r="T309">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U309">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23654,11 +24123,11 @@
         <v/>
       </c>
       <c r="T310">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U310">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23668,11 +24137,11 @@
         <v/>
       </c>
       <c r="T311">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U311">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23682,11 +24151,11 @@
         <v/>
       </c>
       <c r="T312">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U312">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23696,11 +24165,11 @@
         <v/>
       </c>
       <c r="T313">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U313">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23710,11 +24179,11 @@
         <v/>
       </c>
       <c r="T314">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U314">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23724,11 +24193,11 @@
         <v/>
       </c>
       <c r="T315">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U315">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23738,11 +24207,11 @@
         <v/>
       </c>
       <c r="T316">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U316">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23752,11 +24221,11 @@
         <v/>
       </c>
       <c r="T317">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U317">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23766,11 +24235,11 @@
         <v/>
       </c>
       <c r="T318">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U318">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23780,11 +24249,11 @@
         <v/>
       </c>
       <c r="T319">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U319">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>
@@ -23794,11 +24263,11 @@
         <v/>
       </c>
       <c r="T320">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="U320">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>